<commit_message>
algoritimo com parendizado com reforço
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -468,13 +468,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D2" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -485,13 +485,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D3" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -502,13 +502,13 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D4" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
@@ -519,13 +519,13 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D5" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E5" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
@@ -536,13 +536,13 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D6" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
@@ -553,13 +553,13 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D7" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E7" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
@@ -570,13 +570,13 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D8" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
@@ -587,13 +587,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D9" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E9" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
@@ -604,13 +604,13 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D10" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E10" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
@@ -621,13 +621,13 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D11" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12">
@@ -638,13 +638,13 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D12" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E12" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
@@ -655,13 +655,13 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D13" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
@@ -672,13 +672,13 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D14" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15">
@@ -689,13 +689,13 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D15" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
@@ -706,13 +706,13 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D16" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E16" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17">
@@ -723,13 +723,13 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D17" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E17" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18">
@@ -740,13 +740,13 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D18" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E18" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19">
@@ -757,13 +757,13 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D19" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E19" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20">
@@ -774,13 +774,13 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D20" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E20" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21">
@@ -791,13 +791,13 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D21" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E21" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22">
@@ -808,13 +808,13 @@
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D22" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E22" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23">
@@ -825,13 +825,13 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D23" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E23" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24">
@@ -842,13 +842,13 @@
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D24" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E24" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25">
@@ -859,13 +859,13 @@
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D25" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E25" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26">
@@ -876,13 +876,13 @@
         <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D26" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E26" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27">
@@ -893,13 +893,13 @@
         <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D27" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E27" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28">
@@ -910,13 +910,13 @@
         <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D28" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E28" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29">
@@ -927,13 +927,13 @@
         <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D29" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E29" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30">
@@ -944,13 +944,13 @@
         <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D30" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E30" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31">
@@ -961,13 +961,13 @@
         <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D31" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E31" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32">
@@ -978,13 +978,13 @@
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D32" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E32" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33">
@@ -995,13 +995,13 @@
         <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D33" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E33" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34">
@@ -1012,13 +1012,13 @@
         <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D34" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E34" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35">
@@ -1029,13 +1029,13 @@
         <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D35" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E35" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36">
@@ -1046,13 +1046,13 @@
         <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D36" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E36" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37">
@@ -1063,13 +1063,13 @@
         <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D37" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E37" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38">
@@ -1080,13 +1080,13 @@
         <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D38" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E38" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39">
@@ -1097,13 +1097,13 @@
         <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D39" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E39" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40">
@@ -1114,13 +1114,13 @@
         <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D40" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E40" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41">
@@ -1131,13 +1131,13 @@
         <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D41" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E41" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42">
@@ -1148,13 +1148,13 @@
         <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D42" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E42" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43">
@@ -1165,13 +1165,13 @@
         <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D43" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E43" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44">
@@ -1182,13 +1182,13 @@
         <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D44" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E44" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45">
@@ -1199,13 +1199,13 @@
         <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D45" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E45" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46">
@@ -1216,13 +1216,13 @@
         <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D46" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E46" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47">
@@ -1233,13 +1233,13 @@
         <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D47" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E47" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48">
@@ -1250,13 +1250,13 @@
         <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D48" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E48" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49">
@@ -1267,13 +1267,13 @@
         <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D49" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E49" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50">
@@ -1284,13 +1284,13 @@
         <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D50" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E50" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51">
@@ -1301,13 +1301,13 @@
         <v>0</v>
       </c>
       <c r="C51" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D51" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E51" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52">
@@ -1318,13 +1318,13 @@
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D52" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E52" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53">
@@ -1335,13 +1335,13 @@
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D53" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E53" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54">
@@ -1352,13 +1352,13 @@
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D54" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E54" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55">
@@ -1369,13 +1369,13 @@
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D55" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E55" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56">
@@ -1386,13 +1386,13 @@
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D56" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E56" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57">
@@ -1403,13 +1403,13 @@
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D57" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E57" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58">
@@ -1420,13 +1420,13 @@
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D58" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E58" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59">
@@ -1437,13 +1437,13 @@
         <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D59" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E59" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60">
@@ -1454,13 +1454,13 @@
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D60" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E60" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61">
@@ -1471,13 +1471,13 @@
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D61" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E61" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62">
@@ -1488,13 +1488,13 @@
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D62" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E62" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63">
@@ -1505,13 +1505,13 @@
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D63" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E63" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64">
@@ -1522,13 +1522,13 @@
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D64" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E64" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65">
@@ -1539,13 +1539,13 @@
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D65" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E65" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66">
@@ -1556,13 +1556,13 @@
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D66" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E66" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67">
@@ -1573,13 +1573,13 @@
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D67" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E67" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68">
@@ -1590,13 +1590,13 @@
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D68" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E68" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69">
@@ -1607,13 +1607,13 @@
         <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D69" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E69" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70">
@@ -1624,13 +1624,13 @@
         <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D70" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E70" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71">
@@ -1641,13 +1641,13 @@
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D71" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E71" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72">
@@ -1658,13 +1658,13 @@
         <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D72" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E72" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73">
@@ -1675,13 +1675,13 @@
         <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D73" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E73" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74">
@@ -1692,13 +1692,13 @@
         <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D74" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E74" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75">
@@ -1709,13 +1709,13 @@
         <v>0</v>
       </c>
       <c r="C75" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D75" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E75" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76">
@@ -1726,13 +1726,13 @@
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D76" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E76" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77">
@@ -1743,13 +1743,13 @@
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D77" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E77" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78">
@@ -1760,13 +1760,13 @@
         <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D78" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E78" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79">
@@ -1777,13 +1777,13 @@
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D79" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E79" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80">
@@ -1794,13 +1794,13 @@
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D80" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E80" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81">
@@ -1811,13 +1811,13 @@
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D81" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E81" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82">
@@ -1828,13 +1828,13 @@
         <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D82" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E82" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83">
@@ -1845,13 +1845,13 @@
         <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D83" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E83" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84">
@@ -1862,13 +1862,13 @@
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D84" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E84" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85">
@@ -1879,13 +1879,13 @@
         <v>0</v>
       </c>
       <c r="C85" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D85" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E85" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86">
@@ -1896,13 +1896,13 @@
         <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D86" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E86" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87">
@@ -1913,13 +1913,13 @@
         <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D87" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E87" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88">
@@ -1930,13 +1930,13 @@
         <v>0</v>
       </c>
       <c r="C88" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D88" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E88" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89">
@@ -1947,13 +1947,13 @@
         <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D89" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E89" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90">
@@ -1964,13 +1964,13 @@
         <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D90" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E90" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91">
@@ -1981,13 +1981,13 @@
         <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D91" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E91" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92">
@@ -1998,13 +1998,13 @@
         <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D92" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E92" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93">
@@ -2015,13 +2015,13 @@
         <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D93" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E93" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94">
@@ -2032,13 +2032,13 @@
         <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D94" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E94" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95">
@@ -2049,13 +2049,13 @@
         <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D95" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E95" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96">
@@ -2066,13 +2066,13 @@
         <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D96" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E96" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97">
@@ -2083,13 +2083,13 @@
         <v>0</v>
       </c>
       <c r="C97" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D97" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E97" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98">
@@ -2100,13 +2100,13 @@
         <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D98" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E98" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99">
@@ -2117,13 +2117,13 @@
         <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D99" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E99" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100">
@@ -2134,13 +2134,13 @@
         <v>0</v>
       </c>
       <c r="C100" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D100" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E100" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101">
@@ -2151,16 +2151,16 @@
         <v>0</v>
       </c>
       <c r="C101" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D101" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E101" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>